<commit_message>
commented code and added units
</commit_message>
<xml_diff>
--- a/qg/hammered_fit.xlsx
+++ b/qg/hammered_fit.xlsx
@@ -16,22 +16,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
-    <t>amplitude</t>
-  </si>
-  <si>
-    <t>center</t>
-  </si>
-  <si>
-    <t>sigma (width)</t>
-  </si>
-  <si>
-    <t>FWHM</t>
+    <t>amplitude (counts)</t>
+  </si>
+  <si>
+    <t>center (degrees)</t>
+  </si>
+  <si>
+    <t>sigma (width in degrees)</t>
+  </si>
+  <si>
+    <t>FWHM (degrees)</t>
   </si>
   <si>
     <t>model</t>
   </si>
   <si>
-    <t>d</t>
+    <t>d (Angstroms)</t>
   </si>
   <si>
     <t>strain</t>

</xml_diff>